<commit_message>
Track Aws cost estimate file
</commit_message>
<xml_diff>
--- a/data/AWS_Merged.costs.xlsx
+++ b/data/AWS_Merged.costs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bainandcompany-my.sharepoint.com/personal/saloni_vyas_bain_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bainandcompany-my.sharepoint.com/personal/saloni_vyas_bain_com/Documents/Cost-Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{881B377F-BB1A-41A2-B386-6AAE615DB5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1A7BE78-E8AA-4FD8-94FD-8921A966773D}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{881B377F-BB1A-41A2-B386-6AAE615DB5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE5BBC0E-CD43-4505-9544-FA1CE2D217D1}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,13 +605,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A242" sqref="A242:XFD249"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.81640625" customWidth="1"/>
+    <col min="24" max="24" width="25.36328125" customWidth="1"/>
+    <col min="31" max="31" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.35">

</xml_diff>